<commit_message>
update backend and UI
</commit_message>
<xml_diff>
--- a/uploads/en.xlsx
+++ b/uploads/en.xlsx
@@ -434,11 +434,15 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Word</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Meaning</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -456,12 +460,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>('Word', 'hallo')</t>
+          <t>('Word', 'sound')</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>('Meaning', 'dsaf')</t>
+          <t>('Meaning', 'goood')</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
allow users to save file successfully
</commit_message>
<xml_diff>
--- a/uploads/en.xlsx
+++ b/uploads/en.xlsx
@@ -460,12 +460,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>('Word', 'sound')</t>
+          <t>('Word', 'goodbye')</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>('Meaning', 'goood')</t>
+          <t>('Meaning', 'de')</t>
         </is>
       </c>
     </row>

</xml_diff>